<commit_message>
finish parse merged cells
</commit_message>
<xml_diff>
--- a/packages/markitdown/tests/test_files/test.xlsx
+++ b/packages/markitdown/tests/test_files/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamfo\Desktop\test_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Python\markitdown\packages\markitdown\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1161AF-B5D9-455B-AF86-BE2542BA41C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A1A235-D41B-4327-B68F-506D89359520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="737" yWindow="1637" windowWidth="18514" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>ColA</t>
   </si>
@@ -67,17 +67,29 @@
   </si>
   <si>
     <t>6ff4173b-42a5-4784-9b19-f49caff4d93d</t>
+  </si>
+  <si>
+    <t>Group</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Merged Column</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Merged Column 2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -85,8 +97,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -110,12 +129,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -393,15 +424,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -414,8 +445,19 @@
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>89</v>
       </c>
@@ -428,8 +470,17 @@
       <c r="D2">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>70</v>
+      </c>
+      <c r="G2" s="3">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>76</v>
       </c>
@@ -442,8 +493,16 @@
       <c r="D3">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E3" s="3"/>
+      <c r="F3">
+        <v>83</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>60</v>
       </c>
@@ -456,8 +515,16 @@
       <c r="D4">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E4" s="3"/>
+      <c r="F4">
+        <v>71</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>7</v>
       </c>
@@ -470,8 +537,16 @@
       <c r="D5">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E5" s="3"/>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>87</v>
       </c>
@@ -484,8 +559,16 @@
       <c r="D6">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E6" s="3"/>
+      <c r="F6">
+        <v>67</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>23</v>
       </c>
@@ -498,8 +581,16 @@
       <c r="D7">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E7" s="3"/>
+      <c r="F7">
+        <v>42</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7">
+        <v>34.933333333333302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>70</v>
       </c>
@@ -512,8 +603,13 @@
       <c r="D8">
         <v>59</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E8" s="3"/>
+      <c r="F8">
+        <v>34.933333333333302</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>83</v>
       </c>
@@ -526,8 +622,17 @@
       <c r="D9">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E9" s="3">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>28.104761904761901</v>
+      </c>
+      <c r="G9" s="3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>71</v>
       </c>
@@ -540,8 +645,13 @@
       <c r="D10">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E10" s="3"/>
+      <c r="F10">
+        <v>21.2761904761905</v>
+      </c>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>20</v>
       </c>
@@ -554,8 +664,13 @@
       <c r="D11">
         <v>67</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E11" s="3"/>
+      <c r="F11">
+        <v>14.447619047619</v>
+      </c>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>67</v>
       </c>
@@ -568,8 +683,13 @@
       <c r="D12">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E12" s="3"/>
+      <c r="F12">
+        <v>7.6190476190476097</v>
+      </c>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>42</v>
       </c>
@@ -582,8 +702,13 @@
       <c r="D13">
         <v>67</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E13" s="3"/>
+      <c r="F13">
+        <v>0.79047619047621298</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>58</v>
       </c>
@@ -596,8 +721,13 @@
       <c r="D14">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E14" s="3"/>
+      <c r="F14">
+        <v>-6.0380952380951802</v>
+      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>49</v>
       </c>
@@ -610,8 +740,13 @@
       <c r="D15">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E15" s="3"/>
+      <c r="F15">
+        <v>-12.866666666666699</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>82</v>
       </c>
@@ -624,8 +759,13 @@
       <c r="D16">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E16" s="3"/>
+      <c r="F16">
+        <v>-19.6952380952381</v>
+      </c>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>95</v>
       </c>
@@ -638,8 +778,17 @@
       <c r="D17">
         <v>82</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E17" s="3">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>-26.523809523809099</v>
+      </c>
+      <c r="G17" s="3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>50</v>
       </c>
@@ -652,8 +801,13 @@
       <c r="D18">
         <v>86</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E18" s="3"/>
+      <c r="F18">
+        <v>-33.352380952381097</v>
+      </c>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>31</v>
       </c>
@@ -666,8 +820,13 @@
       <c r="D19">
         <v>82</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E19" s="3"/>
+      <c r="F19">
+        <v>-40.1809523809521</v>
+      </c>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>40</v>
       </c>
@@ -680,8 +839,13 @@
       <c r="D20">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E20" s="3"/>
+      <c r="F20">
+        <v>-47.009523809524097</v>
+      </c>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>95</v>
       </c>
@@ -694,8 +858,13 @@
       <c r="D21">
         <v>62</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E21" s="3"/>
+      <c r="F21">
+        <v>-53.8380952380951</v>
+      </c>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>68</v>
       </c>
@@ -708,8 +877,13 @@
       <c r="D22">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E22" s="3"/>
+      <c r="F22">
+        <v>-60.666666666667098</v>
+      </c>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>96</v>
       </c>
@@ -722,8 +896,13 @@
       <c r="D23">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E23" s="3"/>
+      <c r="F23">
+        <v>-67.495238095238093</v>
+      </c>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>87</v>
       </c>
@@ -736,8 +915,24 @@
       <c r="D24">
         <v>80</v>
       </c>
+      <c r="E24" s="3"/>
+      <c r="F24">
+        <v>-74.323809523809103</v>
+      </c>
+      <c r="G24" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="E9:E16"/>
+    <mergeCell ref="E17:E24"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="G9:G16"/>
+    <mergeCell ref="G17:G24"/>
+    <mergeCell ref="G2:G5"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -750,9 +945,9 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -766,7 +961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -780,7 +975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>5</v>
       </c>
@@ -794,7 +989,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>9</v>
       </c>
@@ -808,7 +1003,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>13</v>
       </c>
@@ -823,6 +1018,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>